<commit_message>
WORKING ~ Project Save
</commit_message>
<xml_diff>
--- a/Businesses.xlsx
+++ b/Businesses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,6 +557,1038 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Countertops Unlimited of Texas</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21606 TX-249 B, Houston, TX 77070</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Solis Granite</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Spring, TX 77379</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Simply Solid Surface</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FM 1960, Houston, TX 77090</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Stone Edge Countertops</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10251 Woodedge Dr, Houston, TX 77070</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Keystone Granite and Tile</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>(832) 924-8247</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Precision Countertops</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>13315 Veterans Memorial Dr # 410, Houston, TX 77014</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>R &amp; D Countertops Inc.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11450 Farm to Market 1960 Rd W #116, Houston, TX 77065</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wave Granite and Marble</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>14415 FM 529, Houston, TX 77095</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Houston Granite Remnants</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>16745 Suite B, North Fwy, Houston, TX 77090</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Cypress Granite and Tile</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11223 Jones Rd, Houston, TX 77070</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>StoneStore</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11850 Hempstead Hwy #230, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Rock Fin Countertops, Inc.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5830 Gessner Rd, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Simmons Custom Granite</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5611 W Davis St, Conroe, TX 77304</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>King's Granite &amp; Marble</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2206 Maurine St, Houston, TX 77039</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>New Edge Stone. Inc,</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>4810 Breen Dr, Houston, TX 77086</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>L &amp; M Granite LLC.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1818 Humble Westfield Rd, Houston, TX 77073</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>iGranite</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1808 W Sam Houston Pkwy N, Houston, TX 77043</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Hilltop Stones &amp; Interiors</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>8760 Clay Rd Suite B, Houston, TX 77080</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Galaxy Stone</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>9134 North Fwy, Houston, TX 77037</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>All World Supply &amp; Stone Home Remodel</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>23529 FM1314, Unit B, Porter, TX 77365</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Illusion Stone, Inc</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>7118 Killough St, Houston, TX 77086</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Grand Stone, LLC</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>4909 Weeping Willow Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Majestic Stone Countertops and Flooring</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>8444 Rayson Rd, Houston, TX 77080</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Omni Surfaces North | Marble Granite Quartz Porcelain</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>802 Farm to Market 1960 Rd E, Houston, TX 77073</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Vicostone Houston</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>4710 North Sam Houston Pkwy W #100, Houston, TX 77086</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Epic Granite Countertops</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>5610 Centralcrest St, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Milestone Countertops</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1022 Wirt Rd #308, Houston, TX 77055</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Stone Coverings of Houston</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>11007 W Hardy Rd, Houston, TX 77076</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Granite World</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>303 N Frazier St, Conroe, TX 77301</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>BW Granite Design</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>12430 Hempstead Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Granite Zone</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Nursery Rd, Spring, TX 77380</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>NEW ERA STONE, LLC</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>23142 FM1314, Porter, TX 77365</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Tajams Marble And Granite</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>6429 W Sam Houston Pkwy N, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Euclase Stone Premium Quartz Warehouse</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>5603 Campbell Rd, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>M.O.G. Custom Granite</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>11526 FM 2854 Rd, Conroe, TX 77304</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Glory to GOD, granite countertops in conroe tx , granite &amp; marble services , granite installation</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>16902 Pickering Rd, Conroe, TX 77302</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Maestro Surfaces</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2200 Lauder Rd, Houston, TX 77039</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Durastone Corporation</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>9815 North Fwy, Houston, TX 77037</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Lusso Stone Surfaces - Kitchen Countertop and Flooring</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>lussostonesurfaces.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Yellow Stone Marble &amp; Granite</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1933 Knoll St, Houston, TX 77080</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Elegant Stone Fabrication</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>11981 FM 529 Suite A, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Granite Master</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>4502 Steffani Ln, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Lone Star Countertops</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>11997 FM 3083, Conroe, TX 77301</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Vera Quartz Countertops</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>12642 Hempstead Rd Suite: B, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Target Stone LLC</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>11514 Hempstead Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Kitchen Cabinets and Granite Counter Tops</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>13601 FM 529, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>D&amp;D Granite</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>12390 TX-249 unit A1, Houston, TX 77086</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Top Of The Line Granite &amp; Marble</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>7411 Wright Rd, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>The Granite Crew LLC</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2230 W Little York Rd, Houston, TX 77091</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Jossemmy Stone</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>4830 Ramus St, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Houston Granite Guy</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>houstongraniteguy.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Midwest Tile Marble &amp; Granite</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>10555 Okanella St, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Reborn Granite</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>14730 Hempstead Rd, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SiRi Granite</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>4849 Cranswick Rd building b, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>MSI Houston</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>14777 Chrisman Rd, Houston, TX 77039</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Omni Surfaces Central | Marble Granite Quartz Porcelain</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>8721 Clay Rd STE A, Houston, TX 77080</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Five Stones Countertops &amp; More</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>8938 Spring Branch Dr d1, Houston, TX 77080</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>AXIAL STONES</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>11329 Todd St B, Houston, TX 77055</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Caesarstone Houston</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10650 W Little York Rd, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>City Stone LLC</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>8002 Pinemont Dr, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Vertex Stone Houston</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>5900 Cunningham Rd, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Quartz Surfacing &amp; Stones (Houston, TX)</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>6605 Roxburgh Dr #300, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Ageless Stoneworks Granite &amp; Marble</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1622 Federal Rd, Houston, TX 77015</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Steadfast Stone Crafters, LLC</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>houstonmarblecountertops.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Best Quartz and Granite</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>702 N Sam Houston Pkwy E, Houston, TX 77060</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>roisgranitecountertops</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>8057 Fallbrook Dr, Houston, TX 77064</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>K &amp; N Custom Granite,LLC</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>3421 Bacor Rd, Houston, TX 77084</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Granite Granite, Inc.</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>10410 Hempstead Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Max Marble &amp; Granite Inc.</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>4110 Southerland Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Natural Stone Gallery Inc</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>13202 Murphy Rd, Stafford, TX 77477</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Granite Marble Etc</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>6401 Long Point Rd bldg 600, Houston, TX 77055</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Northwest Granite &amp; Marble</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>11431 Todd St, Houston, TX 77055</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>American Countertop Fabricators</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1500 Brittmoore Rd Suite 504, Houston, TX 77043</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Simply Solid Surface</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>4634 Farm to Market 2920, Spring, TX 77388</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Legacy Granite and Marble Co., Inc</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>6214 Keyko St, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Imperial Granite</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>11126 Neeshaw Dr b9, Houston, TX 77065</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Terry Stone Inc</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>7020 Cotton Dr, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Eagle Stone LLC</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>14120 Hempstead Rd, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Ortega Stone and Tile Creations</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>327 E Roselane St, Houston, TX 77076</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Barron's Granite and Construction - Granite Fabricator, Granite Repair &amp; Installation, Granite Kitchen Countertops</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>tupalo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>QUAN STONE Countertops</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>quowanstone1.wixsite.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>H&amp;V Granite CounterTops Services</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>9414 Bearden Creek Ln, Humble, TX 77396</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Schlitzberger Stone Designs</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>6343 Alder Dr, Houston, TX 77081</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Boeker Countertops of Houston</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>13018 Kaltenbrun Rd #1, Houston, TX 77086</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Sapphire Stone</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>facebook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Pacific Stone Enterprise</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>3375 Old Spanish Trl, Houston, TX 77021</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve exception handling and optimize search attempts
This commit enhances exception handling by adding NoSuchElementException and WebDriverException to the imported exceptions. Additionally, search attempts have been optimized from 50 to 1 for efficiency. The WebDriver now implicitly waits for a maximum duration and a stopping condition has been added if latitude or longitude couldn't be obtained.
</commit_message>
<xml_diff>
--- a/Businesses.xlsx
+++ b/Businesses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B473"/>
+  <dimension ref="A1:B478"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6101,6 +6101,66 @@
         </is>
       </c>
     </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>Cruz Laminates &amp; Countertops</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>5207 Harrisburg Blvd, Houston, TX 77011</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>Sweeney Marble Co</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>2401 Polk St, Houston, TX 77003</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>Victor's Granite Designers</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>3822 Ranch St, Houston, TX 77026</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>Texas Custom Marble &amp; Granite</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>10835 Maple Leaf St, Houston, TX 77016</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>Floor &amp; Decor</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>4330 Dacoma St, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add UI elements and improve data retrieval in main.py
Added GUI elements for user input and improved data retrieval process in the main script. User can now input the search keyword and location directly through the GUI. Enhanced data retrieval by checking latitude and longitude values for validity before proceeding. Also implemented thread support to prevent UI freeze during data retrieval.
</commit_message>
<xml_diff>
--- a/Businesses.xlsx
+++ b/Businesses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B478"/>
+  <dimension ref="A1:B526"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6161,6 +6161,582 @@
         </is>
       </c>
     </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>Natural Stone Inc</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>1929 Dorsett, Houston, TX 77029</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>Laminate Countertops</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>3832 N Shepherd Dr B, Houston, TX 77018</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>Tex-Star Marble and Granite</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>4834 Ramus St, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>BAYOU CITY GRANITE</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>8307 Bauman Rd, Houston, TX 77022</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>Superior Granite</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>205 Meadow Lea Dr, Houston, TX 77022</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>Stone Age Marble &amp; Granite Inc</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>4830 Ramus St, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>AMC Granite &amp; Marble</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>3541 Creekmont Dr, Houston, TX 77091</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>Aprile's Marble &amp; Granite</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>6005 Milwee St # 714, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>Francini Inc. Marble &amp; Granite - Houston</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>7108 Old Katy Rd suite 100, Houston, TX 77024</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>CCH Granite</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>3616 Lumberdale Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>Wilsonart</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>552 Garden Oaks Blvd, Houston, TX 77018</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>A.T. Custom Marble &amp; Granite</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>501 Gulf Bank Rd, Houston, TX 77037</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>Terra Granite Slabs Center</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>12642 Hempstead Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>Marquez Granite And Tile</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>6826 Evans St, Houston, TX 77061</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>Imperial Granite &amp; Cabinets</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>8700 Clay Rd #216, Houston, TX 77080</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>Olympus Marble</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>2141 Bingle Rd, Houston, TX 77055</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>Granite Surfaces</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>8030 Pinemont Dr, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>Museum Flooring Granite Cabinet Factory</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>4004 Gulf St, Houston, TX 77017</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>Quality Countertops Inc</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>1315 Illinois St, South Houston, TX 77587</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>J.K. Granite &amp; Cabinet</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>6601 W Sam Houston Pkwy S, Houston, TX 77072</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>Terraco Stone</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>6411 Ashcroft Dr # A, Houston, TX 77081</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>HTX Custom Countertops</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>10580 Hammerly Blvd #1712, Houston, TX 77043</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>MATERIAL Bespoke Stone + Tile</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>1335 W Gray St Suite 100, Houston, TX 77019</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>B and D Granite and Tile</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>8010 Pinemont Dr, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>Godstone Corp</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>4722 Creekmont Dr, Houston, TX 77091</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>International Granite &amp; Marble (IGM)</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>8017 Pinemont Dr # 300, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>I Q Granite &amp; Flooring Inc</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>8017 Pinemont Dr # 300, Houston, TX 77040</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>I Q Granite &amp; Flooring Inc</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>1306 Washington St, South Houston, TX 77587</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>Toros Countertops &amp; Gabinets</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>1103 Bland St, Houston, TX 77091</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>W R Watson Inc</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>12902 Mula Ln, Stafford, TX 77477</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>C M Custom Marble Design</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>10129 O'Donnell Dr, Houston, TX 77076</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>Vivaldi Lifestyles</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>12614 Hempstead Rd, Houston, TX 77092</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Bath Concepts</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>7026 Old Katy Rd #148, Houston, TX 77024</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>Richmond Granite &amp; Marble</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>16403 W Bellfort Blvd, Sugar Land, TX 77498</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>Space City Kitchen Remodeling Solutions</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>2204a Louisiana St, Houston, TX 77002</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>Roquemore Marble &amp; Granite</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>1291 N Post Oak Rd # 130, Houston, TX 77055</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>The Home Depot</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>1200 Home Depot Blvd, Sunset Valley, TX 78745</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>Anna's Granite Gallery</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>16409 Farm to Market Rd 1325, Austin, TX 78728</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>Capital of Texas Stoneworks</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>9801 Beck Cir, Austin, TX 78758</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>Lackstone Marbles &amp; Granites</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>2200 Denton Dr Suite-114, Austin, TX 78758</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>CitiQuartz Austin LLC</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>10609 Metric Blvd, Austin, TX 78758</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>Langham Group</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>10712 N Lamar Blvd c, Austin, TX 78753</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>J &amp; H Granite, Inc.</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>237 Benelli Dr, Hutto, TX 78634</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>J&amp;L Granite Countertops</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>135 Torchlight Dr, Bastrop, TX 78602</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>PORCELANOSA Austin</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>400 Barton Springs Rd, Austin, TX 78704</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>Floor &amp; Decor</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>12901 N Interstate Hwy 35 #3, Austin, TX 78753</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>The Home Depot</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>1200 Barbara Jordan Blvd, Austin, TX 78723</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>Stone Edge Countertops</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>4502 Steffani Ln, Houston, TX 77041</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>